<commit_message>
added harry potter book 1 & 2
</commit_message>
<xml_diff>
--- a/book_list_2021.xlsx
+++ b/book_list_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13309\Documents\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37B509E-325E-480A-9C03-92867C796172}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A3D0BE-E5C1-48DA-9F0D-B497C8468E00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8D15D3C9-6373-49F1-B09A-BDF89F98B1E4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Title</t>
   </si>
@@ -61,6 +61,27 @@
   </si>
   <si>
     <t>First Time Reading?</t>
+  </si>
+  <si>
+    <t>Harry Potter and the Sorcerers Stone</t>
+  </si>
+  <si>
+    <t>J.K. Rowling</t>
+  </si>
+  <si>
+    <t>fiction;wizards;adventure;harry potter</t>
+  </si>
+  <si>
+    <t>Audio</t>
+  </si>
+  <si>
+    <t>8 Hours 37 Mins</t>
+  </si>
+  <si>
+    <t>Harry Potter and the Chamber of Secrets</t>
+  </si>
+  <si>
+    <t>9 Hours 28 Mins</t>
   </si>
 </sst>
 </file>
@@ -96,8 +117,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A1C975F-FCE4-4625-A25D-CCC6F847164A}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,6 +471,61 @@
         <v>8</v>
       </c>
     </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1">
+        <v>44198</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44198</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1">
+        <v>44198</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
caught up on several additions
</commit_message>
<xml_diff>
--- a/book_list_2021.xlsx
+++ b/book_list_2021.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13309\Documents\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D40BB2-03F1-4146-AF56-A6FDEBAB55B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9069E0F8-F07F-4CBE-89B6-45E01EDBE0E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8D15D3C9-6373-49F1-B09A-BDF89F98B1E4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
   <si>
     <t>Title</t>
   </si>
@@ -100,6 +100,69 @@
   </si>
   <si>
     <t>8 Hours 4 Mins</t>
+  </si>
+  <si>
+    <t>Over Dressed</t>
+  </si>
+  <si>
+    <t>Elizabeth Cline</t>
+  </si>
+  <si>
+    <t>fashion;business;quality;history</t>
+  </si>
+  <si>
+    <t>7 Hours 57 Mins</t>
+  </si>
+  <si>
+    <t>Post Corona</t>
+  </si>
+  <si>
+    <t>Scott Galloway</t>
+  </si>
+  <si>
+    <t>business;coronavirus;big tech;adaptation</t>
+  </si>
+  <si>
+    <t>Hard Copy</t>
+  </si>
+  <si>
+    <t>212 Pages</t>
+  </si>
+  <si>
+    <t>The Immortal Life of Henrietta Lacks</t>
+  </si>
+  <si>
+    <t>Rebecca Skloot</t>
+  </si>
+  <si>
+    <t>science;ethics;cells;biology;biography;henrietta lacks</t>
+  </si>
+  <si>
+    <t>12 Hours 13 Mins</t>
+  </si>
+  <si>
+    <t>Grocery</t>
+  </si>
+  <si>
+    <t>Michael Ruhlman</t>
+  </si>
+  <si>
+    <t>grocery;business;food;health;nutrition</t>
+  </si>
+  <si>
+    <t>11 Hours 9 Mins</t>
+  </si>
+  <si>
+    <t>To Pixar and Beyond</t>
+  </si>
+  <si>
+    <t>Lawrence Levy</t>
+  </si>
+  <si>
+    <t>pixar;business;ipo;disney;strategy</t>
+  </si>
+  <si>
+    <t>248 Pages</t>
   </si>
 </sst>
 </file>
@@ -452,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A1C975F-FCE4-4625-A25D-CCC6F847164A}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,6 +668,151 @@
         <v>0</v>
       </c>
     </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1">
+        <v>44204</v>
+      </c>
+      <c r="D6" s="1">
+        <v>44206</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1">
+        <v>44197</v>
+      </c>
+      <c r="D7" s="1">
+        <v>44207</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="1">
+        <v>44206</v>
+      </c>
+      <c r="D8" s="1">
+        <v>44209</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="1">
+        <v>44209</v>
+      </c>
+      <c r="D9" s="1">
+        <v>44212</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="1">
+        <v>44207</v>
+      </c>
+      <c r="D10" s="1">
+        <v>44213</v>
+      </c>
+      <c r="E10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added harry potter 4, 5, 6 and wizards first rule
</commit_message>
<xml_diff>
--- a/book_list_2021.xlsx
+++ b/book_list_2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\13309\Documents\reading_list\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56EC574-D160-4AE8-9288-195738084722}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8832A86F-B06A-4624-B472-AD8E5C2816A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8D15D3C9-6373-49F1-B09A-BDF89F98B1E4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8D15D3C9-6373-49F1-B09A-BDF89F98B1E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
   <si>
     <t>Title</t>
   </si>
@@ -175,6 +175,36 @@
   </si>
   <si>
     <t>21 Hours 8 Mins</t>
+  </si>
+  <si>
+    <t>Harry Potter and the Goblet of Fire</t>
+  </si>
+  <si>
+    <t>21 Hours 29 Mins</t>
+  </si>
+  <si>
+    <t>Harry Potter and the Order of the Phoenix</t>
+  </si>
+  <si>
+    <t>27 Hours 19 Mins</t>
+  </si>
+  <si>
+    <t>Harry Potter and the Half Blood Prince</t>
+  </si>
+  <si>
+    <t>19 Hours 6 Mins</t>
+  </si>
+  <si>
+    <t>Wizard's First Rule</t>
+  </si>
+  <si>
+    <t>Terry Goodkind</t>
+  </si>
+  <si>
+    <t>fiction;wizards;evil;good;seeker</t>
+  </si>
+  <si>
+    <t>820 Pages</t>
   </si>
 </sst>
 </file>
@@ -527,15 +557,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A1C975F-FCE4-4625-A25D-CCC6F847164A}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="24.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="35.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -564,7 +597,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -593,7 +626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -622,7 +655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -651,7 +684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -680,7 +713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -709,7 +742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -738,7 +771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -767,7 +800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -796,7 +829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -825,7 +858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -851,6 +884,122 @@
         <v>4</v>
       </c>
       <c r="I11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1">
+        <v>44217</v>
+      </c>
+      <c r="D12" s="1">
+        <v>44224</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
+      </c>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="1">
+        <v>44224</v>
+      </c>
+      <c r="D13" s="1">
+        <v>44232</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="I13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="1">
+        <v>44232</v>
+      </c>
+      <c r="D14" s="1">
+        <v>44240</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="1">
+        <v>44214</v>
+      </c>
+      <c r="D15" s="1">
+        <v>44240</v>
+      </c>
+      <c r="E15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H15">
+        <v>4</v>
+      </c>
+      <c r="I15" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added no stopping you
</commit_message>
<xml_diff>
--- a/book_list_2021.xlsx
+++ b/book_list_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8832A86F-B06A-4624-B472-AD8E5C2816A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BB5C3D-BFF7-44F2-BEDC-E3917C156563}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8D15D3C9-6373-49F1-B09A-BDF89F98B1E4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
   <si>
     <t>Title</t>
   </si>
@@ -205,6 +205,21 @@
   </si>
   <si>
     <t>820 Pages</t>
+  </si>
+  <si>
+    <t>No Stopping You</t>
+  </si>
+  <si>
+    <t>Roger Flax</t>
+  </si>
+  <si>
+    <t>self improvement;business;public speaking;success</t>
+  </si>
+  <si>
+    <t>11 Hours 4 Mins</t>
+  </si>
+  <si>
+    <t>Harry Potter and the Deathly Hallows</t>
   </si>
 </sst>
 </file>
@@ -557,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A1C975F-FCE4-4625-A25D-CCC6F847164A}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1003,6 +1018,46 @@
         <v>1</v>
       </c>
     </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="1">
+        <v>44240</v>
+      </c>
+      <c r="D16" s="1">
+        <v>44248</v>
+      </c>
+      <c r="E16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" t="s">
+        <v>60</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="1">
+        <v>44246</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added harry potter 7 and think again
</commit_message>
<xml_diff>
--- a/book_list_2021.xlsx
+++ b/book_list_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BB5C3D-BFF7-44F2-BEDC-E3917C156563}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A559A1-5A88-474E-A4D4-25656B26F07E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8D15D3C9-6373-49F1-B09A-BDF89F98B1E4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="67">
   <si>
     <t>Title</t>
   </si>
@@ -220,6 +220,21 @@
   </si>
   <si>
     <t>Harry Potter and the Deathly Hallows</t>
+  </si>
+  <si>
+    <t>21 Hours 47 Mins</t>
+  </si>
+  <si>
+    <t>Think Again</t>
+  </si>
+  <si>
+    <t>Adam Grant</t>
+  </si>
+  <si>
+    <t>self improvement;business;rethinking</t>
+  </si>
+  <si>
+    <t>6 Hours 40 Mins</t>
   </si>
 </sst>
 </file>
@@ -572,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A1C975F-FCE4-4625-A25D-CCC6F847164A}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1047,7 +1062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>61</v>
       </c>
@@ -1056,6 +1071,53 @@
       </c>
       <c r="C17" s="1">
         <v>44246</v>
+      </c>
+      <c r="D17" s="1">
+        <v>44252</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17">
+        <v>4</v>
+      </c>
+      <c r="I17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="1">
+        <v>44250</v>
+      </c>
+      <c r="D18" s="1">
+        <v>44253</v>
+      </c>
+      <c r="E18" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18">
+        <v>4</v>
+      </c>
+      <c r="I18" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added billion dollar loser
</commit_message>
<xml_diff>
--- a/book_list_2021.xlsx
+++ b/book_list_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zachr\Documents\Personal_Projects\reading_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A559A1-5A88-474E-A4D4-25656B26F07E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EADF655D-BAA6-405B-AF48-5D2A10AF3816}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8D15D3C9-6373-49F1-B09A-BDF89F98B1E4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="71">
   <si>
     <t>Title</t>
   </si>
@@ -235,6 +235,18 @@
   </si>
   <si>
     <t>6 Hours 40 Mins</t>
+  </si>
+  <si>
+    <t>Billion Dollar Loser</t>
+  </si>
+  <si>
+    <t>Reeves Wiedeman</t>
+  </si>
+  <si>
+    <t>business;startups;wework;venture capital;visionary</t>
+  </si>
+  <si>
+    <t>10 Hours 56 Mins</t>
   </si>
 </sst>
 </file>
@@ -587,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A1C975F-FCE4-4625-A25D-CCC6F847164A}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1120,6 +1132,29 @@
         <v>1</v>
       </c>
     </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="1">
+        <v>44253</v>
+      </c>
+      <c r="D19" s="1">
+        <v>44255</v>
+      </c>
+      <c r="E19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>